<commit_message>
update reference file for ZDEMO_EXCEL36
</commit_message>
<xml_diff>
--- a/src/zdemo_excel36.w3mi.data.xlsx
+++ b/src/zdemo_excel36.w3mi.data.xlsx
@@ -453,20 +453,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -513,7 +513,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
@@ -529,7 +529,7 @@
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -540,10 +540,10 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -552,7 +552,7 @@
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -599,17 +599,17 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update reference file for ZDEMO_EXCEL36 (#20)
Co-authored-by: sandraros <34005250+sandraros@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/zdemo_excel36.w3mi.data.xlsx
+++ b/src/zdemo_excel36.w3mi.data.xlsx
@@ -453,20 +453,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -513,7 +513,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
@@ -529,7 +529,7 @@
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -540,10 +540,10 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -552,7 +552,7 @@
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -599,17 +599,17 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>